<commit_message>
aanpassing concepten query, export functie, matrix functionaliteit kenniskluis
</commit_message>
<xml_diff>
--- a/catalogusdata/Concepten/Testdata concepten local.xlsx
+++ b/catalogusdata/Concepten/Testdata concepten local.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lwortel\Documents\Klussen\Kadaster\Deliveries\bp4mc2\catalogusdata\Concepten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\data\ith21266\Documents\Kadaster\bp4mc2\catalogusdata\Concepten\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="URI schema" sheetId="1" r:id="rId1"/>
@@ -596,8 +596,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Neutraal" xfId="2" builtinId="28"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -613,9 +613,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -653,7 +653,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -725,7 +725,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -905,16 +905,16 @@
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="72.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -931,7 +931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -942,7 +942,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -959,7 +959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -976,7 +976,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -993,7 +993,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -1057,7 +1057,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>78</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>78</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>152</v>
       </c>
@@ -1151,7 +1151,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>152</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>122</v>
       </c>
@@ -1176,7 +1176,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>122</v>
       </c>
@@ -1187,67 +1187,67 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D25" s="2"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D26" s="2"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D32" s="2"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D42" s="2"/>
     </row>
   </sheetData>
@@ -1280,21 +1280,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5703125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="43.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>84</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>84</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -1445,7 +1445,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>84</v>
       </c>
@@ -1496,7 +1496,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>84</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -1564,7 +1564,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>78</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>78</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
         <v>78</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
         <v>78</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
         <v>78</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>78</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
         <v>152</v>
       </c>
@@ -1684,7 +1684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>152</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>152</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>152</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>152</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>122</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>122</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>122</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>122</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>122</v>
       </c>
@@ -1837,28 +1837,28 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
     </row>
-    <row r="52" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
       <c r="D52"/>
       <c r="E52"/>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
       <c r="D56" s="9"/>
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="12"/>
       <c r="B57" s="12"/>
       <c r="C57" s="12"/>
@@ -1875,26 +1875,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="30.5703125" customWidth="1"/>
+    <col min="1" max="2" width="30.5546875" customWidth="1"/>
     <col min="3" max="3" width="60" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="31" customWidth="1"/>
-    <col min="7" max="8" width="17.28515625" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" style="5" customWidth="1"/>
-    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="7" max="8" width="17.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="28.88671875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="18.44140625" customWidth="1"/>
     <col min="12" max="12" width="28" style="5" customWidth="1"/>
     <col min="13" max="13" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>124</v>
       </c>
@@ -1962,7 +1962,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>127</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>123</v>
       </c>
@@ -2038,7 +2038,7 @@
       </c>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>60</v>
       </c>
@@ -2074,7 +2074,7 @@
       </c>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>129</v>
       </c>
@@ -2096,7 +2096,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>131</v>
       </c>
@@ -2115,7 +2115,7 @@
       </c>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>132</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>134</v>
       </c>
@@ -2174,7 +2174,7 @@
       </c>
       <c r="K13" s="9"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="K14" s="9"/>
       <c r="M14" s="9"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -2221,7 +2221,7 @@
       <c r="K15" s="9"/>
       <c r="M15" s="9"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
         <v>135</v>
       </c>
@@ -2258,7 +2258,7 @@
       <c r="K17" s="9"/>
       <c r="M17" s="6"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>138</v>
       </c>
@@ -2283,7 +2283,7 @@
       <c r="K18" s="9"/>
       <c r="M18" s="5"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>143</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="K19" s="9"/>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
         <v>136</v>
       </c>
@@ -2342,7 +2342,7 @@
       </c>
       <c r="K21" s="9"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>145</v>
       </c>
@@ -2366,7 +2366,7 @@
       </c>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -2387,7 +2387,7 @@
       </c>
       <c r="K23" s="9"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>141</v>
       </c>
@@ -2402,33 +2402,33 @@
       </c>
       <c r="M24" s="5"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D27" s="3"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="D28" s="3"/>
     </row>
-    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D29" s="3"/>
       <c r="M29" s="5"/>
     </row>
-    <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D30" s="3"/>
       <c r="M30" s="5"/>
     </row>
-    <row r="31" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="D32" s="7"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="D33" s="3"/>
@@ -2445,14 +2445,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="4" width="27.85546875" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="1" max="2" width="27.44140625" customWidth="1"/>
+    <col min="3" max="4" width="27.88671875" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>79</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>148</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>148</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>112</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>112</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>112</v>
       </c>
@@ -2656,7 +2656,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>85</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>85</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>97</v>
       </c>
@@ -2711,7 +2711,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -2744,7 +2744,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>99</v>
       </c>
@@ -2769,14 +2769,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="27.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" customWidth="1"/>
+    <col min="1" max="2" width="27.44140625" customWidth="1"/>
+    <col min="3" max="3" width="27.88671875" customWidth="1"/>
+    <col min="4" max="4" width="31.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>153</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>152</v>
       </c>
@@ -2801,19 +2801,19 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9" s="10"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10" s="10"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11" s="10"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C12" s="10"/>
     </row>
   </sheetData>
@@ -2830,15 +2830,15 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -2852,7 +2852,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>115</v>
       </c>
@@ -2866,7 +2866,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>114</v>
       </c>

</xml_diff>